<commit_message>
added Observer Pattern, MVC_Excel_BSP, and added Observer Pattern to LateX
</commit_message>
<xml_diff>
--- a/MVC/MVC Problem_Beispiel.xlsx
+++ b/MVC/MVC Problem_Beispiel.xlsx
@@ -103,7 +103,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -111,16 +111,51 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -181,7 +216,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$E$5:$E$10</c:f>
+              <c:f>Tabelle1!$C$5:$C$10</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -207,9 +242,9 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$C$5:$C$10</c:f>
+              <c:f>Tabelle1!$A$5:$A$10</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>1610833</c:v>
@@ -242,11 +277,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="146788736"/>
-        <c:axId val="146790272"/>
+        <c:axId val="42115072"/>
+        <c:axId val="42116608"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="146788736"/>
+        <c:axId val="42115072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -256,7 +291,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146790272"/>
+        <c:crossAx val="42116608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -264,7 +299,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="146790272"/>
+        <c:axId val="42116608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -275,7 +310,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146788736"/>
+        <c:crossAx val="42115072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -341,7 +376,7 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$E$5:$E$10</c:f>
+              <c:f>Tabelle1!$C$5:$C$10</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -367,9 +402,9 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$C$5:$C$10</c:f>
+              <c:f>Tabelle1!$A$5:$A$10</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>1610833</c:v>
@@ -401,11 +436,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="146909824"/>
-        <c:axId val="143198848"/>
+        <c:axId val="43271296"/>
+        <c:axId val="43272832"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="146909824"/>
+        <c:axId val="43271296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -426,7 +461,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="143198848"/>
+        <c:crossAx val="43272832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -434,7 +469,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="143198848"/>
+        <c:axId val="43272832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -445,7 +480,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146909824"/>
+        <c:crossAx val="43271296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -682,8 +717,8 @@
               <c:idx val="5"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.31599450228366838"/>
-                  <c:y val="-5.8950431196100488E-2"/>
+                  <c:x val="0.3159945759503463"/>
+                  <c:y val="2.2103407286855139E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -728,7 +763,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$E$5:$E$10</c:f>
+              <c:f>Tabelle1!$C$5:$C$10</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -754,9 +789,9 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$C$5:$C$10</c:f>
+              <c:f>Tabelle1!$A$5:$A$10</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>1610833</c:v>
@@ -808,16 +843,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>666190</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>113459</xdr:rowOff>
+      <xdr:rowOff>180134</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>456640</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1047750</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>70597</xdr:rowOff>
+      <xdr:rowOff>137272</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -838,16 +873,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>3924</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1144657</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>143996</xdr:rowOff>
+      <xdr:rowOff>159440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>419662</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>22412</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>497519</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>143752</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -870,15 +905,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>728942</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1109942</xdr:colOff>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>72277</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>709892</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>530087</xdr:colOff>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>158002</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1190,95 +1225,97 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:E10"/>
+  <dimension ref="A2:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="25.42578125" customWidth="1"/>
-    <col min="4" max="4" width="1.85546875" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
+    <col min="2" max="2" width="1.5703125" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="1" customWidth="1"/>
     <col min="5" max="5" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:5" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="5" t="s">
+    <row r="2" spans="1:3" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
     </row>
-    <row r="4" spans="3:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="C4" s="2" t="s">
+    <row r="4" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="3" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="3:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C5" s="4">
+    <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
         <v>1610833</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="1" t="s">
+      <c r="B5" s="1"/>
+      <c r="C5" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="3:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C6" s="4">
+    <row r="6" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
         <v>796083</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="1" t="s">
+      <c r="B6" s="1"/>
+      <c r="C6" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="3:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C7" s="4">
+    <row r="7" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
         <v>35144</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="1" t="s">
+      <c r="B7" s="1"/>
+      <c r="C7" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="3:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C8" s="4">
+    <row r="8" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
         <v>32177</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="1" t="s">
+      <c r="B8" s="1"/>
+      <c r="C8" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="3:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C9" s="4">
+    <row r="9" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
         <v>25188</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="1" t="s">
+      <c r="B9" s="1"/>
+      <c r="C9" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="3:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C10" s="4">
+    <row r="10" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="5">
         <v>2565</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="1" t="s">
+      <c r="B10" s="1"/>
+      <c r="C10" s="4" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="A2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>

</xml_diff>